<commit_message>
Comment fix, Excel additional data (comments, charts, etc).
</commit_message>
<xml_diff>
--- a/dataset/Experience.xlsx
+++ b/dataset/Experience.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +120,18 @@
   </si>
   <si>
     <t>SoftLink SacralMuseum</t>
+  </si>
+  <si>
+    <t>Code Reuse</t>
+  </si>
+  <si>
+    <t>Development Mode</t>
+  </si>
+  <si>
+    <t>Customer Quality</t>
+  </si>
+  <si>
+    <t>PM Quality</t>
   </si>
 </sst>
 </file>
@@ -163,9 +176,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -181,6 +200,994 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Correlation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Language</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Team</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Size</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Development Mode</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Code Reuse</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Architecture</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Customer Quality</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PM Quality</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$A$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.22540381906681656</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58833261402197501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88199951980579872</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.26789662524016455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.42312093918262578</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20775771477150626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.2546595209141273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.2971228931536446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="837541312"/>
+        <c:axId val="837545120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="837541312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Feature</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="837545120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="837545120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Correlation ratio</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="837541312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>625474</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>565149</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139699</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,7 +1480,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H1" sqref="H1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1341,4 +2348,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>-0.22540381906681656</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.58833261402197501</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.88199951980579872</v>
+      </c>
+      <c r="D2" s="3">
+        <v>-0.26789662524016455</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-0.42312093918262578</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.20775771477150626</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-0.2546595209141273</v>
+      </c>
+      <c r="H2" s="3">
+        <v>-0.2971228931536446</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Learning MSE plot add. Fix dataset (train and test parts) mistake.
</commit_message>
<xml_diff>
--- a/dataset/Experience.xlsx
+++ b/dataset/Experience.xlsx
@@ -164,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -172,19 +172,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -346,11 +362,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="837541312"/>
-        <c:axId val="837545120"/>
+        <c:axId val="282434320"/>
+        <c:axId val="282431056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="837541312"/>
+        <c:axId val="282434320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,7 +463,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="837545120"/>
+        <c:crossAx val="282431056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -455,7 +471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="837545120"/>
+        <c:axId val="282431056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +579,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="837541312"/>
+        <c:crossAx val="282434320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1480,7 +1496,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:L1"/>
+      <selection activeCell="M19" sqref="A1:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1496,814 +1512,814 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>2015</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <f>5*1+1*1+2*1</f>
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
         <f>10738+3052*2</f>
         <v>16842</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
         <v>2</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <f>13*4</f>
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>2016</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
         <f>5*1+3*1+3*1+1*1+1*1</f>
         <v>13</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
         <v>4534</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
         <v>2</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
         <f>5*4</f>
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>2016</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
         <f>5*1+2*1+2*1+1*1+1*1</f>
         <v>11</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
         <v>26892</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <v>20</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>2017</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
         <f>3*1+3*1</f>
         <v>6</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
         <f>15411+16654</f>
         <v>32065</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <v>10</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
         <v>2</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>2018</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <f>3*1+3*1+3*1</f>
         <v>9</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
         <f>972+2029</f>
         <v>3001</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
         <v>35</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
         <v>2</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="4">
         <v>3</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>2018</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <f>3*1+3*1+3*1</f>
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
         <f>203+3700</f>
         <v>3903</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
         <v>30</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
         <v>2</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="4">
         <v>3</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>2018</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <f>3*1+3*1+3*1</f>
         <v>9</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
         <f>2404+946</f>
         <v>3350</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <v>2</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="4">
         <v>3</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="4">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>2018</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <f>5*1+1*1+3*1</f>
         <v>9</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
         <f>728+9400</f>
         <v>10128</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
         <v>20</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
         <v>2</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>2018</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <f>5*1+3*1+1*1</f>
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
         <f>4295+4887+186+2933+2424</f>
         <v>14725</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
         <v>10</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
         <v>2</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="4">
         <v>2</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>2018</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <f>5*1+3*1+1*1</f>
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
         <f>1543*3</f>
         <v>4629</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
         <v>20</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
         <v>2</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>2018</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>5</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <f>5*1+3*1+1*1</f>
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
         <f>1527+70000/10</f>
         <v>8527</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
         <v>50</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1</v>
+      </c>
+      <c r="M12" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>2019</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <f>5*1+1*1+1*1</f>
         <v>7</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
         <f>572*4</f>
         <v>2288</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
         <v>20</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="4">
         <v>2</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>2019</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <f>5*1+5*1+3*1</f>
         <v>13</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
         <v>71308</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
         <v>10</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
         <v>2</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
         <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>2019</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>5</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <f>5*1+3*1</f>
         <v>8</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
         <f>3161</f>
         <v>3161</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
         <v>2</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="4">
         <v>2</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>2019</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>5</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <f>2*1+2*1</f>
         <v>4</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
         <v>3541</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
         <v>60</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
         <v>3</v>
       </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>2019</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>5</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <f>3*1</f>
         <v>3</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
         <f>474</f>
         <v>474</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
         <v>10</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
         <v>3</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="4">
         <v>2</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>2019</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>5</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <f>3*1</f>
         <v>3</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
         <v>1434</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
         <v>50</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
         <v>3</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+      <c r="M18" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>2019</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
         <f>3*1+3*1+1*1</f>
         <v>7</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
         <f>504+1364+703+654+1457</f>
         <v>4682</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
         <v>20</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <v>3</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
         <v>2</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="4">
         <v>16</v>
       </c>
     </row>
@@ -2367,54 +2383,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>-0.22540381906681656</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.58833261402197501</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.88199951980579872</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>-0.26789662524016455</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>-0.42312093918262578</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0.20775771477150626</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>-0.2546595209141273</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>-0.2971228931536446</v>
       </c>
     </row>

</xml_diff>